<commit_message>
Adds timings for slow lloyd's and adjusts names
</commit_message>
<xml_diff>
--- a/misc_figure_code/openmp_algo_speedup_data.xlsx
+++ b/misc_figure_code/openmp_algo_speedup_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t xml:space="preserve">K Centers</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t xml:space="preserve">Elkan’s Speedup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lloyd_slow_seq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lloyd_sl_par</t>
   </si>
 </sst>
 </file>
@@ -58,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -78,6 +85,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,10 +164,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -354,6 +362,87 @@
         <v>1.51797374310873</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>6.41404</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>18.559297</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>100.31866</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>307.145723</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>2.65987</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>7.356104</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>42.23705</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>131.894881</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <f aca="false">B12/B13</f>
+        <v>2.41141108400035</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <f aca="false">C12/C13</f>
+        <v>2.52297914765751</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">D12/D13</f>
+        <v>2.37513415354529</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">E12/E13</f>
+        <v>2.32871602499873</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
speedup data ss update
</commit_message>
<xml_diff>
--- a/misc_figure_code/openmp_algo_speedup_data.xlsx
+++ b/misc_figure_code/openmp_algo_speedup_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t xml:space="preserve">K Centers</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">lloyd_sl_par</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elkan Par Dyn</t>
   </si>
 </sst>
 </file>
@@ -164,10 +167,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -443,6 +446,76 @@
         <v>2.32871602499873</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2.163586</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>10.456343</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>30.44319</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>97.062709</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2.432288</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>6.779244</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>30.706803</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>106.46536</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="n">
+        <f aca="false">SUM(B20:B21)</f>
+        <v>4.595874</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <f aca="false">SUM(C20:C21)</f>
+        <v>17.235587</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">SUM(D20:D21)</f>
+        <v>61.149993</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">SUM(E20:E21)</f>
+        <v>203.528069</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="n">
+        <f aca="false">B22/2</f>
+        <v>2.297937</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <f aca="false">C22/2</f>
+        <v>8.6177935</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">D22/2</f>
+        <v>30.5749965</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">E22/2</f>
+        <v>101.7640345</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>